<commit_message>
added vocabulary of root indicators in D3_clean_all_vaccines
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_ clean_all_vaccines.xlsx
+++ b/i_codebooks/D3_ clean_all_vaccines.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -351,21 +351,6 @@
     <t>Coronavirus</t>
   </si>
   <si>
-    <t>"MCV"
-"DTP"
-"Hib"
-"HepB"
-"Pol"
-"PCV"
-"Varicella"
-"BCG"
-"HPV"
-"RotaC"
-"Meningococcal"
-"Influenza"
-"Coronavirus"</t>
-  </si>
-  <si>
     <t>HPV </t>
   </si>
   <si>
@@ -425,6 +410,21 @@
   </si>
   <si>
     <t>as many as thedoses for that root_indicator, including duplicates</t>
+  </si>
+  <si>
+    <t>"MCV" = measles-containing vaccine
+"DTP" = diphteria-tetatnus-pertussis
+"Hib" = Haemophilus influenzae type B
+"HepB" = Hepatatis B
+"Pol" = Polio
+"PCV" = Pneumococcal conjugate vaccines
+"Varicella" = Varicella
+"BCG" = Bacille Calmette-Guérin vaccine
+"HPV" = Human papillomavirus vaccine
+"RotaC" = Rotavirus
+"Meningococcal" = Meningococcal vaccine
+"Influenza" =Infuenza
+"Coronavirus" = Coronavirus</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1097,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1113,7 +1113,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
@@ -1127,12 +1127,12 @@
         <v>6</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -1143,7 +1143,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1166,11 +1166,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1317,88 +1317,88 @@
         <v>93</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
         <v>110</v>
-      </c>
-      <c r="C9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="30" t="s">
         <v>112</v>
-      </c>
-      <c r="C14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1459,7 +1459,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1822,7 +1822,7 @@
         <v>97</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1924,27 +1924,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2195,32 +2174,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8A1FD8-B49B-4DD5-B035-18D91695717A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93CB37C0-20D2-41C5-B1FB-AE3E189FB0ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2237,4 +2212,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8A1FD8-B49B-4DD5-B035-18D91695717A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
improved example in D3_clean_all_vaccines
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_ clean_all_vaccines.xlsx
+++ b/i_codebooks/D3_ clean_all_vaccines.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="132">
   <si>
     <t>medatata_name</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>doses higher than the vaccine-specific maximum dosage are excluded</t>
-  </si>
-  <si>
-    <t>This dataset contains the records of all the curated doses of all vaccines in the instance listed in Table 4 of the SAP, including the curated covid vaccines. It is obtained by D3_clea_all_vaccines by excluding records that are duplicates or of bad quality</t>
   </si>
   <si>
     <t>label from the VaccO ontology</t>
@@ -407,9 +404,6 @@
   </si>
   <si>
     <t>root indicators for all persons in the instance</t>
-  </si>
-  <si>
-    <t>as many as thedoses for that root_indicator, including duplicates</t>
   </si>
   <si>
     <t>"MCV" = measles-containing vaccine
@@ -425,6 +419,42 @@
 "Meningococcal" = Meningococcal vaccine
 "Influenza" =Infuenza
 "Coronavirus" = Coronavirus</t>
+  </si>
+  <si>
+    <t>DIP-HIB-PER-POL-TET</t>
+  </si>
+  <si>
+    <t>DIP-HIB-PER-POL-TETATC</t>
+  </si>
+  <si>
+    <t>DIP-HIB-PER-POL-TETVXTYPE</t>
+  </si>
+  <si>
+    <t>Pol</t>
+  </si>
+  <si>
+    <t>vx_record_date</t>
+  </si>
+  <si>
+    <t>vx_dose</t>
+  </si>
+  <si>
+    <t>vx_manufacturer</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>P004</t>
+  </si>
+  <si>
+    <t>as many as the doses for that root_indicator, including duplicates</t>
+  </si>
+  <si>
+    <t>This dataset contains the records of all the curated doses of all vaccines in the instance listed in Table 4 of the SAP, including the curated covid vaccines. It is obtained from the original conceptsets datastes by replicating each vaccination record as many times as the indicators that it is used for, see the first example in the tab Example: a record with Vacco Id DIP-HIB-PER-POL-TET is replicated 3 times, once per the indicator DPT, once per the indicator HiB, and once for the indicator Pol. Then, each record is labelled with various exclusion citeria, most importantly, records with dats 30 daya apart form a previous record as marked as 'duplicates'. In the next step, all the record labelled as 'removed row' will be removed</t>
   </si>
 </sst>
 </file>
@@ -509,7 +539,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -528,8 +558,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -676,9 +718,20 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -687,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -752,11 +805,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1074,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,15 +1174,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1113,7 +1190,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
@@ -1127,12 +1204,12 @@
         <v>6</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
-        <v>117</v>
+      <c r="A7" s="32" t="s">
+        <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -1143,7 +1220,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1166,11 +1243,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,16 +1357,16 @@
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
         <v>24</v>
@@ -1297,108 +1374,108 @@
     </row>
     <row r="7" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" t="s">
         <v>109</v>
-      </c>
-      <c r="C9" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="30" t="s">
         <v>111</v>
-      </c>
-      <c r="C14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1477,197 +1554,197 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1677,244 +1754,838 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <pane xSplit="11" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" style="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="G1" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="H1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="I1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="G1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L1" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="24">
         <v>44318</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="24">
+        <v>44318</v>
+      </c>
+      <c r="D2" s="23">
         <v>1</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E2" s="23"/>
+      <c r="F2" s="24">
+        <v>44318</v>
+      </c>
+      <c r="G2" s="23">
+        <v>1</v>
+      </c>
+      <c r="H2" s="23"/>
+      <c r="I2" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="25">
+        <v>0</v>
+      </c>
+      <c r="M2" s="25">
+        <v>0</v>
+      </c>
+      <c r="N2" s="25">
+        <v>0</v>
+      </c>
+      <c r="O2" s="25">
+        <v>0</v>
+      </c>
+      <c r="P2" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="24">
         <v>44404</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="24">
+        <v>44404</v>
+      </c>
+      <c r="D3" s="23">
         <v>2</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="23"/>
+      <c r="F3" s="24">
+        <v>44404</v>
+      </c>
+      <c r="G3" s="23">
+        <v>2</v>
+      </c>
+      <c r="H3" s="23"/>
+      <c r="I3" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="25">
+        <v>0</v>
+      </c>
+      <c r="M3" s="25">
+        <v>0</v>
+      </c>
+      <c r="N3" s="25">
+        <v>0</v>
+      </c>
+      <c r="O3" s="25">
+        <v>0</v>
+      </c>
+      <c r="P3" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="24">
+        <v>44318</v>
+      </c>
+      <c r="C4" s="24">
+        <v>44318</v>
+      </c>
+      <c r="D4" s="23">
+        <v>1</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24">
+        <v>44318</v>
+      </c>
+      <c r="G4" s="23">
+        <v>1</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="L4" s="25">
+        <v>0</v>
+      </c>
+      <c r="M4" s="25">
+        <v>0</v>
+      </c>
+      <c r="N4" s="25">
+        <v>0</v>
+      </c>
+      <c r="O4" s="25">
+        <v>0</v>
+      </c>
+      <c r="P4" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="24">
+        <v>44404</v>
+      </c>
+      <c r="C5" s="24">
+        <v>44404</v>
+      </c>
+      <c r="D5" s="23">
+        <v>2</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="24">
+        <v>44404</v>
+      </c>
+      <c r="G5" s="23">
+        <v>2</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="L5" s="25">
+        <v>0</v>
+      </c>
+      <c r="M5" s="25">
+        <v>0</v>
+      </c>
+      <c r="N5" s="25">
+        <v>0</v>
+      </c>
+      <c r="O5" s="25">
+        <v>0</v>
+      </c>
+      <c r="P5" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="24">
+        <v>44318</v>
+      </c>
+      <c r="C6" s="24">
+        <v>44318</v>
+      </c>
+      <c r="D6" s="23">
+        <v>1</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24">
+        <v>44318</v>
+      </c>
+      <c r="G6" s="23">
+        <v>1</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25">
+        <v>0</v>
+      </c>
+      <c r="M6" s="25">
+        <v>0</v>
+      </c>
+      <c r="N6" s="25">
+        <v>0</v>
+      </c>
+      <c r="O6" s="25">
+        <v>0</v>
+      </c>
+      <c r="P6" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="24">
+        <v>44404</v>
+      </c>
+      <c r="C7" s="24">
+        <v>44404</v>
+      </c>
+      <c r="D7" s="23">
+        <v>2</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24">
+        <v>44404</v>
+      </c>
+      <c r="G7" s="23">
+        <v>2</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25">
+        <v>0</v>
+      </c>
+      <c r="M7" s="25">
+        <v>0</v>
+      </c>
+      <c r="N7" s="25">
+        <v>0</v>
+      </c>
+      <c r="O7" s="25">
+        <v>0</v>
+      </c>
+      <c r="P7" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="28">
+        <v>44428</v>
+      </c>
+      <c r="C8" s="28">
+        <v>44428</v>
+      </c>
+      <c r="D8" s="27">
+        <v>1</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="28">
+        <v>44428</v>
+      </c>
+      <c r="G8" s="27">
+        <v>1</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" s="22">
+        <v>0</v>
+      </c>
+      <c r="M8" s="22">
+        <v>0</v>
+      </c>
+      <c r="N8" s="22">
+        <v>0</v>
+      </c>
+      <c r="O8" s="22">
+        <v>0</v>
+      </c>
+      <c r="P8" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="21">
+        <v>44407</v>
+      </c>
+      <c r="C9" s="21">
+        <v>44407</v>
+      </c>
+      <c r="D9" s="20">
+        <v>2</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="21">
+        <v>44407</v>
+      </c>
+      <c r="G9" s="20">
+        <v>2</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="22">
+        <v>0</v>
+      </c>
+      <c r="M9" s="22">
+        <v>0</v>
+      </c>
+      <c r="N9" s="22">
+        <v>0</v>
+      </c>
+      <c r="O9" s="22">
+        <v>0</v>
+      </c>
+      <c r="P9" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="21">
+        <v>44772</v>
+      </c>
+      <c r="C10" s="21">
+        <v>44772</v>
+      </c>
+      <c r="D10" s="20">
+        <v>1</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21">
+        <v>44772</v>
+      </c>
+      <c r="G10" s="20">
+        <v>1</v>
+      </c>
+      <c r="H10" s="20"/>
+      <c r="I10" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="J10" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="K10" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="22">
+        <v>0</v>
+      </c>
+      <c r="M10" s="22">
+        <v>0</v>
+      </c>
+      <c r="N10" s="22">
+        <v>0</v>
+      </c>
+      <c r="O10" s="22">
+        <v>0</v>
+      </c>
+      <c r="P10" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="24">
+        <v>44197</v>
+      </c>
+      <c r="C11" s="24">
+        <v>44197</v>
+      </c>
+      <c r="D11" s="23">
+        <v>1</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="24">
+        <v>44197</v>
+      </c>
+      <c r="G11" s="23">
+        <v>1</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="L11" s="25">
+        <v>0</v>
+      </c>
+      <c r="M11" s="25">
+        <v>0</v>
+      </c>
+      <c r="N11" s="25">
+        <v>0</v>
+      </c>
+      <c r="O11" s="25">
+        <v>0</v>
+      </c>
+      <c r="P11" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="24">
+        <v>44221</v>
+      </c>
+      <c r="C12" s="24">
+        <v>44221</v>
+      </c>
+      <c r="D12" s="23">
+        <v>2</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="24">
+        <v>44221</v>
+      </c>
+      <c r="G12" s="23">
+        <v>2</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K12" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="L12" s="25">
+        <v>0</v>
+      </c>
+      <c r="M12" s="25">
+        <v>0</v>
+      </c>
+      <c r="N12" s="25">
+        <v>0</v>
+      </c>
+      <c r="O12" s="25">
+        <v>0</v>
+      </c>
+      <c r="P12" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="24">
+        <v>44287</v>
+      </c>
+      <c r="C13" s="24">
+        <v>44287</v>
+      </c>
+      <c r="D13" s="23">
+        <v>3</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="24">
+        <v>44287</v>
+      </c>
+      <c r="G13" s="23">
+        <v>3</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="L13" s="25">
+        <v>0</v>
+      </c>
+      <c r="M13" s="25">
+        <v>0</v>
+      </c>
+      <c r="N13" s="25">
+        <v>0</v>
+      </c>
+      <c r="O13" s="25">
+        <v>0</v>
+      </c>
+      <c r="P13" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="24">
+        <v>44481</v>
+      </c>
+      <c r="C14" s="24">
+        <v>44481</v>
+      </c>
+      <c r="D14" s="23">
+        <v>4</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="24">
+        <v>44481</v>
+      </c>
+      <c r="G14" s="23">
+        <v>4</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="L14" s="25">
+        <v>0</v>
+      </c>
+      <c r="M14" s="25">
+        <v>0</v>
+      </c>
+      <c r="N14" s="25">
+        <v>0</v>
+      </c>
+      <c r="O14" s="25">
+        <v>0</v>
+      </c>
+      <c r="P14" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="34">
+        <v>44318</v>
+      </c>
+      <c r="C15" s="34">
+        <v>44318</v>
+      </c>
+      <c r="D15" s="33">
+        <v>1</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34">
+        <v>44318</v>
+      </c>
+      <c r="G15" s="33">
+        <v>1</v>
+      </c>
+      <c r="H15" s="33"/>
+      <c r="I15" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="45" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="28">
-        <v>44428</v>
-      </c>
-      <c r="C4" s="27">
+      <c r="K15" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="L15" s="39">
+        <v>0</v>
+      </c>
+      <c r="M15" s="39">
+        <v>0</v>
+      </c>
+      <c r="N15" s="39">
+        <v>0</v>
+      </c>
+      <c r="O15" s="39">
+        <v>0</v>
+      </c>
+      <c r="P15" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="34">
+        <v>44404</v>
+      </c>
+      <c r="C16" s="34">
+        <v>44318</v>
+      </c>
+      <c r="D16" s="33">
         <v>1</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="29" t="s">
+      <c r="E16" s="33"/>
+      <c r="F16" s="34">
+        <v>44404</v>
+      </c>
+      <c r="G16" s="33">
+        <v>1</v>
+      </c>
+      <c r="H16" s="33"/>
+      <c r="I16" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="21">
-        <v>44407</v>
-      </c>
-      <c r="C5" s="20">
-        <v>2</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="21">
-        <v>44772</v>
-      </c>
-      <c r="C6" s="20">
+      <c r="J16" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="L16" s="39">
+        <v>0</v>
+      </c>
+      <c r="M16" s="39">
+        <v>0</v>
+      </c>
+      <c r="N16" s="39">
+        <v>0</v>
+      </c>
+      <c r="O16" s="40">
         <v>1</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="24">
-        <v>44197</v>
-      </c>
-      <c r="C7" s="23">
+      <c r="P16" s="40">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="24">
-        <v>44221</v>
-      </c>
-      <c r="C8" s="23">
-        <v>2</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="24">
-        <v>44287</v>
-      </c>
-      <c r="C9" s="23">
-        <v>3</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="G9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="24">
-        <v>44481</v>
-      </c>
-      <c r="C10" s="23">
-        <v>4</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="G10" t="s">
-        <v>100</v>
+      <c r="Q16" s="39" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1924,6 +2595,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2174,28 +2866,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8A1FD8-B49B-4DD5-B035-18D91695717A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93CB37C0-20D2-41C5-B1FB-AE3E189FB0ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2212,29 +2908,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8A1FD8-B49B-4DD5-B035-18D91695717A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>